<commit_message>
update policy quota api
</commit_message>
<xml_diff>
--- a/excel/policyNumber.xlsx
+++ b/excel/policyNumber.xlsx
@@ -14,78 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>policyId</t>
   </si>
   <si>
-    <t>100-0000020</t>
-  </si>
-  <si>
-    <t>100-0000021</t>
-  </si>
-  <si>
-    <t>100-0000022</t>
-  </si>
-  <si>
-    <t>100-0000023</t>
-  </si>
-  <si>
-    <t>100-0000024</t>
-  </si>
-  <si>
-    <t>100-0000025</t>
-  </si>
-  <si>
-    <t>100-0000026</t>
-  </si>
-  <si>
-    <t>100-0000027</t>
-  </si>
-  <si>
-    <t>100-0000028</t>
-  </si>
-  <si>
-    <t>100-0000029</t>
-  </si>
-  <si>
-    <t>100-0000030</t>
-  </si>
-  <si>
-    <t>100-0000031</t>
-  </si>
-  <si>
-    <t>100-0000032</t>
-  </si>
-  <si>
-    <t>100-0000033</t>
-  </si>
-  <si>
-    <t>100-0000034</t>
-  </si>
-  <si>
-    <t>100-0000035</t>
-  </si>
-  <si>
-    <t>100-0000036</t>
-  </si>
-  <si>
-    <t>100-0000037</t>
-  </si>
-  <si>
-    <t>100-0000038</t>
-  </si>
-  <si>
-    <t>100-0000039</t>
-  </si>
-  <si>
-    <t>100-0000040</t>
-  </si>
-  <si>
-    <t>100-0000041</t>
-  </si>
-  <si>
-    <t>100-0000042</t>
+    <t>100-0000043</t>
+  </si>
+  <si>
+    <t>100-0000044</t>
+  </si>
+  <si>
+    <t>100-0000045</t>
+  </si>
+  <si>
+    <t>100-0000046</t>
+  </si>
+  <si>
+    <t>100-0000047</t>
+  </si>
+  <si>
+    <t>100-0000048</t>
+  </si>
+  <si>
+    <t>100-0000049</t>
+  </si>
+  <si>
+    <t>100-0000050</t>
+  </si>
+  <si>
+    <t>100-0000051</t>
+  </si>
+  <si>
+    <t>100-0000052</t>
   </si>
 </sst>
 </file>
@@ -427,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,71 +451,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>